<commit_message>
adding COG estimate for rotating machine DER
</commit_message>
<xml_diff>
--- a/HCA/SimpleRVC.xlsx
+++ b/HCA/SimpleRVC.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IEEE\p1729\HostingCapacityTF\TestFeeder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8452528-07C1-4F2A-9BB8-A9E4279D8A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D488EF1A-0780-4ADB-BB55-E4E29AB59C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7880" yWindow="4040" windowWidth="28800" windowHeight="15450" xr2:uid="{7D6E8C32-CACD-498D-B92F-BBC7DE0016F8}"/>
+    <workbookView xWindow="4010" yWindow="7160" windowWidth="22660" windowHeight="12780" xr2:uid="{7D6E8C32-CACD-498D-B92F-BBC7DE0016F8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RVC" sheetId="1" r:id="rId1"/>
+    <sheet name="LineCodes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DP">Sheet1!$B$9</definedName>
-    <definedName name="DQ">Sheet1!$B$10</definedName>
-    <definedName name="RG">Sheet1!$E$7</definedName>
-    <definedName name="Term1">Sheet1!$E$9</definedName>
-    <definedName name="Term2">Sheet1!$E$10</definedName>
-    <definedName name="VT">Sheet1!$B$8</definedName>
-    <definedName name="X">Sheet1!$F$7</definedName>
-    <definedName name="XG">Sheet1!$F$7</definedName>
+    <definedName name="DP">RVC!$B$9</definedName>
+    <definedName name="DQ">RVC!$B$10</definedName>
+    <definedName name="RG">RVC!$E$7</definedName>
+    <definedName name="Term1">RVC!$E$9</definedName>
+    <definedName name="Term2">RVC!$E$10</definedName>
+    <definedName name="VT">RVC!$B$8</definedName>
+    <definedName name="X">RVC!$F$7</definedName>
+    <definedName name="XG">RVC!$F$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Linecode</t>
   </si>
@@ -160,33 +161,6 @@
   </si>
   <si>
     <t>VT [V]</t>
-  </si>
-  <si>
-    <r>
-      <t>Z pcc [</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>W</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]</t>
-    </r>
   </si>
   <si>
     <r>
@@ -258,6 +232,219 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> [VAR]</t>
+    </r>
+  </si>
+  <si>
+    <t>R0/mi</t>
+  </si>
+  <si>
+    <t>X0/mi</t>
+  </si>
+  <si>
+    <r>
+      <t>R0 [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>X0 [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Z1 pcc [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Z0 pcc [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>r11</t>
+  </si>
+  <si>
+    <t>r22</t>
+  </si>
+  <si>
+    <t>r31</t>
+  </si>
+  <si>
+    <t>r32</t>
+  </si>
+  <si>
+    <t>r33</t>
+  </si>
+  <si>
+    <t>r21</t>
+  </si>
+  <si>
+    <t>x11</t>
+  </si>
+  <si>
+    <t>x21</t>
+  </si>
+  <si>
+    <t>x22</t>
+  </si>
+  <si>
+    <t>x31</t>
+  </si>
+  <si>
+    <t>x32</t>
+  </si>
+  <si>
+    <t>x33</t>
+  </si>
+  <si>
+    <t>Xs</t>
+  </si>
+  <si>
+    <t>Xm</t>
+  </si>
+  <si>
+    <t>Rs</t>
+  </si>
+  <si>
+    <t>Rm</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>X0</t>
+  </si>
+  <si>
+    <t>Check R0/X1 &lt; 1?</t>
+  </si>
+  <si>
+    <t>Check X0/X1 &lt; 3?</t>
+  </si>
+  <si>
+    <t>(pass)</t>
+  </si>
+  <si>
+    <t>(fail)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Y Xfmr</t>
     </r>
   </si>
 </sst>
@@ -351,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -365,6 +552,11 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1843010-0F75-4F32-9C3A-9E872FD46926}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -693,7 +885,7 @@
     <col min="5" max="5" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -712,8 +904,14 @@
       <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="J1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>20</v>
       </c>
@@ -734,8 +932,19 @@
         <f>D2*$B2*$B2/$A2</f>
         <v>0.62200359999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="I2" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="3">
+        <f>E2</f>
+        <v>7.7750449999999999E-2</v>
+      </c>
+      <c r="K2" s="3">
+        <f>F2</f>
+        <v>0.62200359999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -748,97 +957,166 @@
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>0.30599999999999999</v>
-      </c>
-      <c r="C4">
-        <v>0.61339999999999995</v>
+      <c r="B4" s="3">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.63200000000000001</v>
       </c>
       <c r="D4" s="5">
         <v>6600</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" ref="E4:E5" si="0">$D4/5280*B4</f>
-        <v>0.38250000000000001</v>
+        <v>0.38</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" ref="F4:F5" si="1">$D4/5280*C4</f>
-        <v>0.76674999999999993</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>0.79</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.744</v>
+      </c>
+      <c r="J4" s="3">
+        <f>H4*$D4/5280</f>
+        <v>0.78999999999999992</v>
+      </c>
+      <c r="K4" s="3">
+        <f>I4*$D4/5280</f>
+        <v>2.1799999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>1.6879999999999999</v>
       </c>
-      <c r="C5">
-        <v>0.83899999999999997</v>
+      <c r="C5" s="3">
+        <v>0.84799999999999998</v>
       </c>
       <c r="D5" s="5">
-        <v>5300</v>
+        <v>3960</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>1.6943939393939396</v>
+        <v>1.266</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
-        <v>0.8421780303030304</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2.3919999999999999</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2.5680000000000001</v>
+      </c>
+      <c r="J5" s="3">
+        <f>H5*$D5/5280</f>
+        <v>1.794</v>
+      </c>
+      <c r="K5" s="3">
+        <f>I5*$D5/5280</f>
+        <v>1.9260000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6">
-        <v>5.4390000000000001</v>
-      </c>
-      <c r="C6">
-        <v>0.83699999999999997</v>
+      <c r="B6" s="3">
+        <v>5.4386999999999999</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.83730000000000004</v>
       </c>
       <c r="D6" s="5">
-        <v>0</v>
+        <v>1320</v>
       </c>
       <c r="E6">
         <f>$D6/5280*B6</f>
-        <v>0</v>
+        <v>1.359675</v>
       </c>
       <c r="F6">
         <f>$D6/5280*C6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>0.20932500000000001</v>
+      </c>
+      <c r="H6" s="3">
+        <v>5.9946999999999999</v>
+      </c>
+      <c r="I6" s="3">
+        <v>3.0253000000000001</v>
+      </c>
+      <c r="J6" s="3">
+        <f>H6*$D6/5280</f>
+        <v>1.498675</v>
+      </c>
+      <c r="K6" s="3">
+        <f>I6*$D6/5280</f>
+        <v>0.75632500000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E7" s="3">
         <f>SUM(E2:E6)</f>
-        <v>2.1546443893939395</v>
+        <v>3.08342545</v>
       </c>
       <c r="F7" s="3">
         <f>SUM(F2:F6)</f>
-        <v>2.2309316303030302</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>2.2573286000000001</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="3">
+        <f>SUM(J2:J6)</f>
+        <v>4.16042545</v>
+      </c>
+      <c r="K7" s="3">
+        <f>SUM(K2:K6)</f>
+        <v>5.4843286000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="5">
         <v>12470</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="H8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="12">
+        <f>K7/F7</f>
+        <v>2.4295659036969628</v>
+      </c>
+      <c r="K8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6">
         <v>922000</v>
@@ -848,12 +1126,22 @@
       </c>
       <c r="E9" s="10">
         <f>VT*VT+RG*DP+XG*DQ</f>
-        <v>157487482.12702122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>158343818.2649</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="12">
+        <f>J7/F7</f>
+        <v>1.8430747964651668</v>
+      </c>
+      <c r="K9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="6">
         <v>0</v>
@@ -863,16 +1151,16 @@
       </c>
       <c r="E10" s="10">
         <f>XG*DP-RG*DQ</f>
-        <v>2056918.9631393938</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>2081256.9692000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="7">
-        <f>SQRT(Term1*Term1+Term2*Term1)/VT/VT-1</f>
-        <v>1.93677671627559E-2</v>
+        <f>SQRT(Term1*Term1+Term2*Term2)/VT/VT-1</f>
+        <v>1.8370283399112841E-2</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>13</v>
@@ -886,4 +1174,338 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2C2BD4-7D2A-4E5E-8468-ECE48D3E7507}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1.92</v>
+      </c>
+      <c r="D2" s="3">
+        <v>5.6239999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.112</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.9359999999999999</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5.6280000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.104</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.112</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.9119999999999999</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1.008</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.4239999999999999</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.5680000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.752</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.4079999999999999</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.5640000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.67600000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1.024</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1.4319999999999999</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.5680000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="3">
+        <f>(B2+B4+B7)/3</f>
+        <v>0.41333333333333333</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" ref="C14:D14" si="0">(C2+C4+C7)/3</f>
+        <v>1.9226666666666665</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>5.6239999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="3">
+        <f>(B3+B5+B6)/3</f>
+        <v>0.10933333333333334</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" ref="C15:D15" si="1">(C3+C5+C6)/3</f>
+        <v>0.23466666666666666</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="1"/>
+        <v>0.18533333333333335</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="3">
+        <f>(B8+B10+B13)/3</f>
+        <v>1.0026666666666666</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" ref="C16:D16" si="2">(C8+C10+C13)/3</f>
+        <v>1.4213333333333331</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="2"/>
+        <v>1.5666666666666667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="3">
+        <f>(B9+B11+B12)/3</f>
+        <v>0.3706666666666667</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" ref="C17:D17" si="3">(C9+C11+C12)/3</f>
+        <v>0.57333333333333336</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="3"/>
+        <v>0.72933333333333328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="11">
+        <f>B14-B15</f>
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="C18" s="11">
+        <f t="shared" ref="C18:D18" si="4">C14-C15</f>
+        <v>1.6879999999999999</v>
+      </c>
+      <c r="D18" s="11">
+        <f t="shared" si="4"/>
+        <v>5.4386666666666663</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="11">
+        <f>B16-B17</f>
+        <v>0.6319999999999999</v>
+      </c>
+      <c r="C19" s="11">
+        <f t="shared" ref="C19:D19" si="5">C16-C17</f>
+        <v>0.84799999999999975</v>
+      </c>
+      <c r="D19" s="11">
+        <f t="shared" si="5"/>
+        <v>0.83733333333333337</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="11">
+        <f>B14+2*B15</f>
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="C20" s="11">
+        <f t="shared" ref="C20:D20" si="6">C14+2*C15</f>
+        <v>2.3919999999999999</v>
+      </c>
+      <c r="D20" s="11">
+        <f t="shared" si="6"/>
+        <v>5.9946666666666664</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="11">
+        <f>B16+2*B17</f>
+        <v>1.744</v>
+      </c>
+      <c r="C21" s="11">
+        <f t="shared" ref="C21:D21" si="7">C16+2*C17</f>
+        <v>2.5679999999999996</v>
+      </c>
+      <c r="D21" s="11">
+        <f t="shared" si="7"/>
+        <v>3.0253333333333332</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added short circuit angle example
</commit_message>
<xml_diff>
--- a/HCA/SimpleRVC.xlsx
+++ b/HCA/SimpleRVC.xlsx
@@ -1,28 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IEEE\p1729\HostingCapacityTF\TestFeeder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\IEEE1729DynamicsTF\HCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D488EF1A-0780-4ADB-BB55-E4E29AB59C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B994CFFC-B8CB-4250-B391-23E9AC920F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4010" yWindow="7160" windowWidth="22660" windowHeight="12780" xr2:uid="{7D6E8C32-CACD-498D-B92F-BBC7DE0016F8}"/>
+    <workbookView xWindow="5210" yWindow="2950" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{7D6E8C32-CACD-498D-B92F-BBC7DE0016F8}"/>
   </bookViews>
   <sheets>
     <sheet name="RVC" sheetId="1" r:id="rId1"/>
-    <sheet name="LineCodes" sheetId="2" r:id="rId2"/>
+    <sheet name="FaultsPOC" sheetId="3" r:id="rId2"/>
+    <sheet name="LineCodes" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="DP">RVC!$B$9</definedName>
     <definedName name="DQ">RVC!$B$10</definedName>
+    <definedName name="IbaseDER">FaultsPOC!$H$3</definedName>
+    <definedName name="IBRAng">FaultsPOC!$I$2</definedName>
+    <definedName name="IscIBR">FaultsPOC!$H$2</definedName>
+    <definedName name="IscMach">FaultsPOC!$H$1</definedName>
+    <definedName name="MachAng">FaultsPOC!$I$1</definedName>
     <definedName name="RG">RVC!$E$7</definedName>
+    <definedName name="Sder">FaultsPOC!$B$2</definedName>
     <definedName name="Term1">RVC!$E$9</definedName>
     <definedName name="Term2">RVC!$E$10</definedName>
     <definedName name="VT">RVC!$B$8</definedName>
+    <definedName name="VTf">FaultsPOC!$B$1</definedName>
     <definedName name="X">RVC!$F$7</definedName>
     <definedName name="XG">RVC!$F$7</definedName>
   </definedNames>
@@ -47,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t>Linecode</t>
   </si>
@@ -446,6 +454,97 @@
       </rPr>
       <t>Y Xfmr</t>
     </r>
+  </si>
+  <si>
+    <t>S [VA]</t>
+  </si>
+  <si>
+    <r>
+      <t>Zslgf [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>Mag</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>Islgf [A]</t>
+  </si>
+  <si>
+    <t>Re</t>
+  </si>
+  <si>
+    <t>Im</t>
+  </si>
+  <si>
+    <t>Imach [A]</t>
+  </si>
+  <si>
+    <t>Mach Isc</t>
+  </si>
+  <si>
+    <t>IBR Isc</t>
+  </si>
+  <si>
+    <t>Ibase DER</t>
+  </si>
+  <si>
+    <t>Iibr [A]</t>
+  </si>
+  <si>
+    <t>IBR</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>Adding Current Magnitudes:</t>
+  </si>
+  <si>
+    <t>Adding Phasors:</t>
+  </si>
+  <si>
+    <t>Magnitude Errors:</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Increment</t>
+  </si>
+  <si>
+    <t>At POC</t>
+  </si>
+  <si>
+    <t>At Sub</t>
+  </si>
+  <si>
+    <t>POC</t>
+  </si>
+  <si>
+    <t>Sub</t>
   </si>
 </sst>
 </file>
@@ -455,7 +554,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -510,8 +609,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -521,6 +627,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,7 +650,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -557,6 +669,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,10 +992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1843010-0F75-4F32-9C3A-9E872FD46926}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -885,7 +1005,7 @@
     <col min="5" max="5" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -911,7 +1031,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:15">
       <c r="A2" s="5">
         <v>20</v>
       </c>
@@ -944,7 +1064,7 @@
         <v>0.62200359999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -963,8 +1083,14 @@
       <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="N3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -975,15 +1101,15 @@
         <v>0.63200000000000001</v>
       </c>
       <c r="D4" s="5">
-        <v>6600</v>
+        <v>2000</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" ref="E4:E5" si="0">$D4/5280*B4</f>
-        <v>0.38</v>
+        <v>0.11515151515151514</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" ref="F4:F5" si="1">$D4/5280*C4</f>
-        <v>0.79</v>
+        <v>0.23939393939393938</v>
       </c>
       <c r="H4" s="3">
         <v>0.63200000000000001</v>
@@ -992,15 +1118,21 @@
         <v>1.744</v>
       </c>
       <c r="J4" s="3">
-        <f>H4*$D4/5280</f>
-        <v>0.78999999999999992</v>
+        <f t="shared" ref="J4:K6" si="2">H4*$D4/5280</f>
+        <v>0.23939393939393938</v>
       </c>
       <c r="K4" s="3">
-        <f>I4*$D4/5280</f>
-        <v>2.1799999999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <f t="shared" si="2"/>
+        <v>0.66060606060606064</v>
+      </c>
+      <c r="N4">
+        <v>6600</v>
+      </c>
+      <c r="O4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1011,15 +1143,15 @@
         <v>0.84799999999999998</v>
       </c>
       <c r="D5" s="5">
-        <v>3960</v>
+        <v>0</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>1.266</v>
+        <v>0</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
-        <v>0.63600000000000001</v>
+        <v>0</v>
       </c>
       <c r="H5" s="3">
         <v>2.3919999999999999</v>
@@ -1028,15 +1160,21 @@
         <v>2.5680000000000001</v>
       </c>
       <c r="J5" s="3">
-        <f>H5*$D5/5280</f>
-        <v>1.794</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="K5" s="3">
-        <f>I5*$D5/5280</f>
-        <v>1.9260000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>3960</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1047,15 +1185,15 @@
         <v>0.83730000000000004</v>
       </c>
       <c r="D6" s="5">
-        <v>1320</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f>$D6/5280*B6</f>
-        <v>1.359675</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <f>$D6/5280*C6</f>
-        <v>0.20932500000000001</v>
+        <v>0</v>
       </c>
       <c r="H6" s="3">
         <v>5.9946999999999999</v>
@@ -1064,39 +1202,45 @@
         <v>3.0253000000000001</v>
       </c>
       <c r="J6" s="3">
-        <f>H6*$D6/5280</f>
-        <v>1.498675</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="K6" s="3">
-        <f>I6*$D6/5280</f>
-        <v>0.75632500000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>1320</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="3">
         <f>SUM(E2:E6)</f>
-        <v>3.08342545</v>
+        <v>0.19290196515151514</v>
       </c>
       <c r="F7" s="3">
         <f>SUM(F2:F6)</f>
-        <v>2.2573286000000001</v>
+        <v>0.86139753939393937</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J7" s="3">
         <f>SUM(J2:J6)</f>
-        <v>4.16042545</v>
+        <v>0.31714438939393941</v>
       </c>
       <c r="K7" s="3">
         <f>SUM(K2:K6)</f>
-        <v>5.4843286000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>1.2826096606060606</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1108,38 +1252,44 @@
       </c>
       <c r="J8" s="12">
         <f>K7/F7</f>
-        <v>2.4295659036969628</v>
+        <v>1.4889869101651683</v>
       </c>
       <c r="K8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:15">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="6">
-        <v>922000</v>
+        <v>5000000</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="10">
         <f>VT*VT+RG*DP+XG*DQ</f>
-        <v>158343818.2649</v>
+        <v>156465409.82575756</v>
       </c>
       <c r="H9" t="s">
         <v>44</v>
       </c>
       <c r="J9" s="12">
         <f>J7/F7</f>
-        <v>1.8430747964651668</v>
+        <v>0.36817424579257019</v>
       </c>
       <c r="K9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="N9" s="19">
+        <v>922000</v>
+      </c>
+      <c r="O9" s="19">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1151,23 +1301,23 @@
       </c>
       <c r="E10" s="10">
         <f>XG*DP-RG*DQ</f>
-        <v>2081256.9692000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>4306987.6969696973</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="7">
         <f>SQRT(Term1*Term1+Term2*Term2)/VT/VT-1</f>
-        <v>1.8370283399112841E-2</v>
+        <v>6.58373897155351E-3</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="9">
         <f>SQRT(DP*DP+DQ*DQ)/VT/SQRT(3)</f>
-        <v>42.687806591245788</v>
+        <v>231.49569734948909</v>
       </c>
     </row>
   </sheetData>
@@ -1177,6 +1327,369 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD079EA4-2A18-469F-85DC-EDBA86EFCFA2}">
+  <dimension ref="A1:R23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="9.90625" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5">
+        <v>12470</v>
+      </c>
+      <c r="G1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="5">
+        <v>5</v>
+      </c>
+      <c r="I1" s="5">
+        <v>-85</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="6">
+        <v>5000000</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="M2" s="19">
+        <v>922000</v>
+      </c>
+      <c r="Q2" s="19">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="16">
+        <v>0.19290196515151514</v>
+      </c>
+      <c r="C3" s="16">
+        <v>0.86139753939393937</v>
+      </c>
+      <c r="D3" s="3">
+        <f>SQRT(B3*B3+C3*C3)</f>
+        <v>0.88273262601608293</v>
+      </c>
+      <c r="E3" s="12">
+        <f>DEGREES(ATAN2(B3,C3))</f>
+        <v>77.377398644331976</v>
+      </c>
+      <c r="G3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="12">
+        <f>Sder/SQRT(3)/VTf</f>
+        <v>231.49569734948909</v>
+      </c>
+      <c r="M3">
+        <v>3.08342545</v>
+      </c>
+      <c r="N3">
+        <v>2.2573286000000001</v>
+      </c>
+      <c r="Q3">
+        <v>0.19290196515151514</v>
+      </c>
+      <c r="R3">
+        <v>0.86139753939393937</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0.31714438939393941</v>
+      </c>
+      <c r="C4" s="16">
+        <v>1.2826096606060606</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" ref="D4:D5" si="0">SQRT(B4*B4+C4*C4)</f>
+        <v>1.3212373387109708</v>
+      </c>
+      <c r="E4" s="12">
+        <f t="shared" ref="E4:E5" si="1">DEGREES(ATAN2(B4,C4))</f>
+        <v>76.111340974296184</v>
+      </c>
+      <c r="M4">
+        <v>4.16042545</v>
+      </c>
+      <c r="N4">
+        <v>5.4843286000000004</v>
+      </c>
+      <c r="Q4">
+        <v>0.31714438939393941</v>
+      </c>
+      <c r="R4">
+        <v>1.2826096606060606</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="3">
+        <f>2*(B3+B4)/3</f>
+        <v>0.34003090303030303</v>
+      </c>
+      <c r="C5" s="3">
+        <f>2*(C3+C4)/3</f>
+        <v>1.4293381333333333</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4692271827108361</v>
+      </c>
+      <c r="E5" s="12">
+        <f t="shared" si="1"/>
+        <v>76.618416652034867</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="B6" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="12">
+        <f>VTf/SQRT(3)/D5</f>
+        <v>4900.2345869417559</v>
+      </c>
+      <c r="C7" s="12">
+        <f>-E5</f>
+        <v>-76.618416652034867</v>
+      </c>
+      <c r="D7" s="12">
+        <f>$B7*COS(RADIANS($C7))</f>
+        <v>1134.0868255539658</v>
+      </c>
+      <c r="E7" s="12">
+        <f>$B7*SIN(RADIANS($C7))</f>
+        <v>-4767.194780913107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8">
+        <f>IscMach*IbaseDER</f>
+        <v>1157.4784867474455</v>
+      </c>
+      <c r="C8" s="17">
+        <f>MachAng</f>
+        <v>-85</v>
+      </c>
+      <c r="D8" s="12">
+        <f t="shared" ref="D8:D9" si="2">$B8*COS(RADIANS($C8))</f>
+        <v>100.88089722690898</v>
+      </c>
+      <c r="E8" s="12">
+        <f t="shared" ref="E8:E9" si="3">$B8*SIN(RADIANS($C8))</f>
+        <v>-1153.0739316530619</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <f>IscIBR*IbaseDER</f>
+        <v>277.79483681938689</v>
+      </c>
+      <c r="C9">
+        <f>IBRAng</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="12">
+        <f t="shared" si="2"/>
+        <v>277.79483681938689</v>
+      </c>
+      <c r="E9" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="12">
+        <f>B7+B8</f>
+        <v>6057.7130736892013</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="12">
+        <f>B7+B9</f>
+        <v>5178.0294237611424</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="B16" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="12">
+        <f>D7+D8</f>
+        <v>1234.9677227808747</v>
+      </c>
+      <c r="C17" s="12">
+        <f>E7+E8</f>
+        <v>-5920.2687125661687</v>
+      </c>
+      <c r="D17" s="12">
+        <f>SQRT(B17*B17+C17*C17)</f>
+        <v>6047.7042673481037</v>
+      </c>
+      <c r="E17" s="12">
+        <f>DEGREES(ATAN2(B17,C17))</f>
+        <v>-78.217071600558768</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="12">
+        <f>D7+D9</f>
+        <v>1411.8816623733528</v>
+      </c>
+      <c r="C18" s="12">
+        <f>E7+E9</f>
+        <v>-4767.194780913107</v>
+      </c>
+      <c r="D18" s="12">
+        <f>SQRT(B18*B18+C18*C18)</f>
+        <v>4971.8764976325901</v>
+      </c>
+      <c r="E18" s="12">
+        <f>DEGREES(ATAN2(B18,C18))</f>
+        <v>-73.50249456935623</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="18">
+        <f>B12/D17-1</f>
+        <v>1.6549761527089313E-3</v>
+      </c>
+      <c r="C22" s="18">
+        <f>(B12-B7)/(D17-B7)-1</f>
+        <v>8.7225017898104884E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="18">
+        <f>B13/D18-1</f>
+        <v>4.1463806718995189E-2</v>
+      </c>
+      <c r="C23" s="18">
+        <f>(B13-B7)/(D18-B7)-1</f>
+        <v>2.8775464548704046</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2C2BD4-7D2A-4E5E-8468-ECE48D3E7507}">
   <dimension ref="A1:D21"/>
   <sheetViews>

</xml_diff>

<commit_message>
correcting errors in Zslgf
</commit_message>
<xml_diff>
--- a/HCA/SimpleRVC.xlsx
+++ b/HCA/SimpleRVC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\IEEE1729DynamicsTF\HCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B994CFFC-B8CB-4250-B391-23E9AC920F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0EF6E7-AC96-4156-A5C5-CAA398525D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5210" yWindow="2950" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{7D6E8C32-CACD-498D-B92F-BBC7DE0016F8}"/>
+    <workbookView xWindow="22420" yWindow="3870" windowWidth="16440" windowHeight="14000" xr2:uid="{7D6E8C32-CACD-498D-B92F-BBC7DE0016F8}"/>
   </bookViews>
   <sheets>
     <sheet name="RVC" sheetId="1" r:id="rId1"/>
@@ -650,7 +650,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -669,12 +669,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -696,9 +694,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -736,7 +734,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -842,7 +840,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -984,7 +982,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -994,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1843010-0F75-4F32-9C3A-9E872FD46926}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1101,15 +1099,15 @@
         <v>0.63200000000000001</v>
       </c>
       <c r="D4" s="5">
-        <v>2000</v>
+        <v>6600</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" ref="E4:E5" si="0">$D4/5280*B4</f>
-        <v>0.11515151515151514</v>
+        <v>0.38</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" ref="F4:F5" si="1">$D4/5280*C4</f>
-        <v>0.23939393939393938</v>
+        <v>0.79</v>
       </c>
       <c r="H4" s="3">
         <v>0.63200000000000001</v>
@@ -1119,11 +1117,11 @@
       </c>
       <c r="J4" s="3">
         <f t="shared" ref="J4:K6" si="2">H4*$D4/5280</f>
-        <v>0.23939393939393938</v>
+        <v>0.78999999999999992</v>
       </c>
       <c r="K4" s="3">
         <f t="shared" si="2"/>
-        <v>0.66060606060606064</v>
+        <v>2.1799999999999997</v>
       </c>
       <c r="N4">
         <v>6600</v>
@@ -1143,15 +1141,15 @@
         <v>0.84799999999999998</v>
       </c>
       <c r="D5" s="5">
-        <v>0</v>
+        <v>3960</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.266</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="H5" s="3">
         <v>2.3919999999999999</v>
@@ -1161,11 +1159,11 @@
       </c>
       <c r="J5" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.794</v>
       </c>
       <c r="K5" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.9260000000000002</v>
       </c>
       <c r="N5">
         <v>3960</v>
@@ -1185,15 +1183,15 @@
         <v>0.83730000000000004</v>
       </c>
       <c r="D6" s="5">
-        <v>0</v>
+        <v>1320</v>
       </c>
       <c r="E6">
         <f>$D6/5280*B6</f>
-        <v>0</v>
+        <v>1.359675</v>
       </c>
       <c r="F6">
         <f>$D6/5280*C6</f>
-        <v>0</v>
+        <v>0.20932500000000001</v>
       </c>
       <c r="H6" s="3">
         <v>5.9946999999999999</v>
@@ -1203,11 +1201,11 @@
       </c>
       <c r="J6" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.498675</v>
       </c>
       <c r="K6" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.75632500000000003</v>
       </c>
       <c r="N6">
         <v>1320</v>
@@ -1222,22 +1220,22 @@
       </c>
       <c r="E7" s="3">
         <f>SUM(E2:E6)</f>
-        <v>0.19290196515151514</v>
+        <v>3.08342545</v>
       </c>
       <c r="F7" s="3">
         <f>SUM(F2:F6)</f>
-        <v>0.86139753939393937</v>
+        <v>2.2573286000000001</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J7" s="3">
         <f>SUM(J2:J6)</f>
-        <v>0.31714438939393941</v>
+        <v>4.16042545</v>
       </c>
       <c r="K7" s="3">
         <f>SUM(K2:K6)</f>
-        <v>1.2826096606060606</v>
+        <v>5.4843286000000004</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1252,7 +1250,7 @@
       </c>
       <c r="J8" s="12">
         <f>K7/F7</f>
-        <v>1.4889869101651683</v>
+        <v>2.4295659036969628</v>
       </c>
       <c r="K8" t="s">
         <v>46</v>
@@ -1263,29 +1261,29 @@
         <v>15</v>
       </c>
       <c r="B9" s="6">
-        <v>5000000</v>
+        <v>922000</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="10">
         <f>VT*VT+RG*DP+XG*DQ</f>
-        <v>156465409.82575756</v>
+        <v>158343818.2649</v>
       </c>
       <c r="H9" t="s">
         <v>44</v>
       </c>
       <c r="J9" s="12">
         <f>J7/F7</f>
-        <v>0.36817424579257019</v>
+        <v>1.8430747964651668</v>
       </c>
       <c r="K9" t="s">
         <v>47</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="17">
         <v>922000</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="17">
         <v>5000000</v>
       </c>
     </row>
@@ -1301,7 +1299,7 @@
       </c>
       <c r="E10" s="10">
         <f>XG*DP-RG*DQ</f>
-        <v>4306987.6969696973</v>
+        <v>2081256.9692000002</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1310,14 +1308,14 @@
       </c>
       <c r="B12" s="7">
         <f>SQRT(Term1*Term1+Term2*Term2)/VT/VT-1</f>
-        <v>6.58373897155351E-3</v>
+        <v>1.8370283399112841E-2</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="9">
         <f>SQRT(DP*DP+DQ*DQ)/VT/SQRT(3)</f>
-        <v>231.49569734948909</v>
+        <v>42.687806591245788</v>
       </c>
     </row>
   </sheetData>
@@ -1330,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD079EA4-2A18-469F-85DC-EDBA86EFCFA2}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1372,10 +1370,10 @@
       <c r="B2" s="6">
         <v>5000000</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>52</v>
       </c>
       <c r="G2" t="s">
@@ -1387,10 +1385,10 @@
       <c r="I2" s="5">
         <v>0</v>
       </c>
-      <c r="M2" s="19">
+      <c r="M2" s="17">
         <v>922000</v>
       </c>
-      <c r="Q2" s="19">
+      <c r="Q2" s="17">
         <v>5000000</v>
       </c>
     </row>
@@ -1398,10 +1396,10 @@
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="15">
         <v>0.19290196515151514</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="15">
         <v>0.86139753939393937</v>
       </c>
       <c r="D3" s="3">
@@ -1436,10 +1434,10 @@
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="15">
         <v>0.31714438939393941</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <v>1.2826096606060606</v>
       </c>
       <c r="D4" s="3">
@@ -1464,37 +1462,37 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="14" t="s">
+      <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5" s="3">
-        <f>2*(B3+B4)/3</f>
-        <v>0.34003090303030303</v>
+        <f>(2*B3+B4)/3</f>
+        <v>0.23431610656565657</v>
       </c>
       <c r="C5" s="3">
-        <f>2*(C3+C4)/3</f>
-        <v>1.4293381333333333</v>
+        <f>(2*C3+C4)/3</f>
+        <v>1.0018015797979798</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="0"/>
-        <v>1.4692271827108361</v>
+        <v>1.0288393669965279</v>
       </c>
       <c r="E5" s="12">
         <f t="shared" si="1"/>
-        <v>76.618416652034867</v>
+        <v>76.835476832401341</v>
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1504,19 +1502,19 @@
       </c>
       <c r="B7" s="12">
         <f>VTf/SQRT(3)/D5</f>
-        <v>4900.2345869417559</v>
+        <v>6997.7472555430813</v>
       </c>
       <c r="C7" s="12">
         <f>-E5</f>
-        <v>-76.618416652034867</v>
+        <v>-76.835476832401341</v>
       </c>
       <c r="D7" s="12">
         <f>$B7*COS(RADIANS($C7))</f>
-        <v>1134.0868255539658</v>
+        <v>1593.7229311472265</v>
       </c>
       <c r="E7" s="12">
         <f>$B7*SIN(RADIANS($C7))</f>
-        <v>-4767.194780913107</v>
+        <v>-6813.8472151345031</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -1527,7 +1525,7 @@
         <f>IscMach*IbaseDER</f>
         <v>1157.4784867474455</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="12">
         <f>MachAng</f>
         <v>-85</v>
       </c>
@@ -1572,7 +1570,7 @@
       </c>
       <c r="B12" s="12">
         <f>B7+B8</f>
-        <v>6057.7130736892013</v>
+        <v>8155.2257422905268</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1581,7 +1579,7 @@
       </c>
       <c r="B13" s="12">
         <f>B7+B9</f>
-        <v>5178.0294237611424</v>
+        <v>7275.5420923624679</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -1590,16 +1588,16 @@
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="14" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1609,19 +1607,19 @@
       </c>
       <c r="B17" s="12">
         <f>D7+D8</f>
-        <v>1234.9677227808747</v>
+        <v>1694.6038283741354</v>
       </c>
       <c r="C17" s="12">
         <f>E7+E8</f>
-        <v>-5920.2687125661687</v>
+        <v>-7966.9211467875648</v>
       </c>
       <c r="D17" s="12">
         <f>SQRT(B17*B17+C17*C17)</f>
-        <v>6047.7042673481037</v>
+        <v>8145.15283431018</v>
       </c>
       <c r="E17" s="12">
         <f>DEGREES(ATAN2(B17,C17))</f>
-        <v>-78.217071600558768</v>
+        <v>-77.991863922075368</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1630,19 +1628,19 @@
       </c>
       <c r="B18" s="12">
         <f>D7+D9</f>
-        <v>1411.8816623733528</v>
+        <v>1871.5177679666135</v>
       </c>
       <c r="C18" s="12">
         <f>E7+E9</f>
-        <v>-4767.194780913107</v>
+        <v>-6813.8472151345031</v>
       </c>
       <c r="D18" s="12">
         <f>SQRT(B18*B18+C18*C18)</f>
-        <v>4971.8764976325901</v>
+        <v>7066.1936448848437</v>
       </c>
       <c r="E18" s="12">
         <f>DEGREES(ATAN2(B18,C18))</f>
-        <v>-73.50249456935623</v>
+        <v>-74.641654114679824</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1651,10 +1649,10 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1662,26 +1660,26 @@
       <c r="A22" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="16">
         <f>B12/D17-1</f>
-        <v>1.6549761527089313E-3</v>
-      </c>
-      <c r="C22" s="18">
+        <v>1.2366751349239813E-3</v>
+      </c>
+      <c r="C22" s="16">
         <f>(B12-B7)/(D17-B7)-1</f>
-        <v>8.7225017898104884E-3</v>
+        <v>8.778855678190256E-3</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="16">
         <f>B13/D18-1</f>
-        <v>4.1463806718995189E-2</v>
-      </c>
-      <c r="C23" s="18">
+        <v>2.9626763431422454E-2</v>
+      </c>
+      <c r="C23" s="16">
         <f>(B13-B7)/(D18-B7)-1</f>
-        <v>2.8775464548704046</v>
+        <v>3.0585754703921371</v>
       </c>
     </row>
   </sheetData>
@@ -1694,7 +1692,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
more description for Figure B.6
</commit_message>
<xml_diff>
--- a/HCA/SimpleRVC.xlsx
+++ b/HCA/SimpleRVC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\IEEE1729DynamicsTF\HCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0EF6E7-AC96-4156-A5C5-CAA398525D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A62258-C981-4C5A-9FB9-3EBFABF55128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22420" yWindow="3870" windowWidth="16440" windowHeight="14000" xr2:uid="{7D6E8C32-CACD-498D-B92F-BBC7DE0016F8}"/>
+    <workbookView xWindow="790" yWindow="2770" windowWidth="12510" windowHeight="15590" activeTab="1" xr2:uid="{7D6E8C32-CACD-498D-B92F-BBC7DE0016F8}"/>
   </bookViews>
   <sheets>
     <sheet name="RVC" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
   <si>
     <t>Linecode</t>
   </si>
@@ -490,9 +490,6 @@
     <t>Angle</t>
   </si>
   <si>
-    <t>Islgf [A]</t>
-  </si>
-  <si>
     <t>Re</t>
   </si>
   <si>
@@ -514,27 +511,6 @@
     <t>Iibr [A]</t>
   </si>
   <si>
-    <t>IBR</t>
-  </si>
-  <si>
-    <t>Machine</t>
-  </si>
-  <si>
-    <t>Adding Current Magnitudes:</t>
-  </si>
-  <si>
-    <t>Adding Phasors:</t>
-  </si>
-  <si>
-    <t>Magnitude Errors:</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Increment</t>
-  </si>
-  <si>
     <t>At POC</t>
   </si>
   <si>
@@ -545,14 +521,67 @@
   </si>
   <si>
     <t>Sub</t>
+  </si>
+  <si>
+    <t>Rslgf</t>
+  </si>
+  <si>
+    <t>Xslgf</t>
+  </si>
+  <si>
+    <t>Igrid_slgf [A]</t>
+  </si>
+  <si>
+    <t>Adding Current Magnitudes for Total Islgf:</t>
+  </si>
+  <si>
+    <t>Adding Phasors for Total Islgf:</t>
+  </si>
+  <si>
+    <t>w/ IBR DER</t>
+  </si>
+  <si>
+    <t>w/ Machine DER</t>
+  </si>
+  <si>
+    <t>Errors from Adding Magnitudes vs. Phasor Arithmetic:</t>
+  </si>
+  <si>
+    <t>in Total Ilsgf</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>D I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>slgf</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -650,7 +679,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -675,6 +704,7 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -992,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1843010-0F75-4F32-9C3A-9E872FD46926}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1082,10 +1112,10 @@
         <v>18</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="O3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1328,16 +1358,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD079EA4-2A18-469F-85DC-EDBA86EFCFA2}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
     <col min="2" max="2" width="9.90625" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="9.81640625" customWidth="1"/>
     <col min="5" max="5" width="10.54296875" customWidth="1"/>
+    <col min="6" max="6" width="2.453125" customWidth="1"/>
+    <col min="9" max="9" width="6.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -1348,7 +1381,7 @@
         <v>12470</v>
       </c>
       <c r="G1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" s="5">
         <v>5</v>
@@ -1357,10 +1390,10 @@
         <v>-85</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -1377,7 +1410,7 @@
         <v>52</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H2" s="5">
         <v>1.2</v>
@@ -1411,7 +1444,7 @@
         <v>77.377398644331976</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H3" s="12">
         <f>Sder/SQRT(3)/VTf</f>
@@ -1490,15 +1523,15 @@
         <v>52</v>
       </c>
       <c r="D6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B7" s="12">
         <f>VTf/SQRT(3)/D5</f>
@@ -1519,7 +1552,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8">
         <f>IscMach*IbaseDER</f>
@@ -1540,7 +1573,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9">
         <f>IscIBR*IbaseDER</f>
@@ -1561,12 +1594,12 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B12" s="12">
         <f>B7+B8</f>
@@ -1575,7 +1608,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B13" s="12">
         <f>B7+B9</f>
@@ -1584,15 +1617,15 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="B16" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>51</v>
@@ -1603,7 +1636,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B17" s="12">
         <f>D7+D8</f>
@@ -1624,7 +1657,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B18" s="12">
         <f>D7+D9</f>
@@ -1645,20 +1678,20 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" s="14" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B22" s="16">
         <f>B12/D17-1</f>
@@ -1671,7 +1704,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B23" s="16">
         <f>B13/D18-1</f>
@@ -1684,15 +1717,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2C2BD4-7D2A-4E5E-8468-ECE48D3E7507}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2015,6 +2049,40 @@
         <v>3.0253333333333332</v>
       </c>
     </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="18">
+        <f>(2*B18+B20)/3</f>
+        <v>0.41333333333333333</v>
+      </c>
+      <c r="C23" s="18">
+        <f t="shared" ref="C23:D23" si="8">(2*C18+C20)/3</f>
+        <v>1.9226666666666665</v>
+      </c>
+      <c r="D23" s="18">
+        <f t="shared" si="8"/>
+        <v>5.6239999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="18">
+        <f>(2*B19+B21)/3</f>
+        <v>1.0026666666666666</v>
+      </c>
+      <c r="C24" s="18">
+        <f t="shared" ref="C24:D24" si="9">(2*C19+C21)/3</f>
+        <v>1.4213333333333331</v>
+      </c>
+      <c r="D24" s="18">
+        <f t="shared" si="9"/>
+        <v>1.5666666666666667</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
saved with inputs to match Figures B.4 and B.6
</commit_message>
<xml_diff>
--- a/HCA/SimpleRVC.xlsx
+++ b/HCA/SimpleRVC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\IEEE1729DynamicsTF\HCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A62258-C981-4C5A-9FB9-3EBFABF55128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BCFCB9-6F53-4E83-A4C8-61FDD46F6C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="790" yWindow="2770" windowWidth="12510" windowHeight="15590" activeTab="1" xr2:uid="{7D6E8C32-CACD-498D-B92F-BBC7DE0016F8}"/>
+    <workbookView xWindow="5340" yWindow="4290" windowWidth="14660" windowHeight="11160" xr2:uid="{7D6E8C32-CACD-498D-B92F-BBC7DE0016F8}"/>
   </bookViews>
   <sheets>
     <sheet name="RVC" sheetId="1" r:id="rId1"/>
@@ -581,7 +581,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -704,7 +704,7 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1022,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1843010-0F75-4F32-9C3A-9E872FD46926}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1031,6 +1031,8 @@
     <col min="1" max="1" width="9.26953125" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.453125" customWidth="1"/>
+    <col min="12" max="12" width="2.54296875" customWidth="1"/>
+    <col min="13" max="13" width="2.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -1114,7 +1116,7 @@
       <c r="N3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1215,11 +1217,11 @@
       <c r="D6" s="5">
         <v>1320</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <f>$D6/5280*B6</f>
         <v>1.359675</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <f>$D6/5280*C6</f>
         <v>0.20932500000000001</v>
       </c>
@@ -1356,10 +1358,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD079EA4-2A18-469F-85DC-EDBA86EFCFA2}">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1371,9 +1373,13 @@
     <col min="5" max="5" width="10.54296875" customWidth="1"/>
     <col min="6" max="6" width="2.453125" customWidth="1"/>
     <col min="9" max="9" width="6.7265625" customWidth="1"/>
+    <col min="10" max="10" width="2.36328125" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" customWidth="1"/>
+    <col min="12" max="12" width="7.1796875" customWidth="1"/>
+    <col min="13" max="13" width="2.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1389,14 +1395,14 @@
       <c r="I1" s="5">
         <v>-85</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:15">
       <c r="A2" s="4" t="s">
         <v>49</v>
       </c>
@@ -1418,30 +1424,30 @@
       <c r="I2" s="5">
         <v>0</v>
       </c>
-      <c r="M2" s="17">
+      <c r="K2" s="17">
         <v>922000</v>
       </c>
-      <c r="Q2" s="17">
+      <c r="N2" s="17">
         <v>5000000</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="15">
-        <v>0.19290196515151514</v>
+        <v>0.19289999999999999</v>
       </c>
       <c r="C3" s="15">
-        <v>0.86139753939393937</v>
+        <v>0.86140000000000005</v>
       </c>
       <c r="D3" s="3">
         <f>SQRT(B3*B3+C3*C3)</f>
-        <v>0.88273262601608293</v>
+        <v>0.88273459771326512</v>
       </c>
       <c r="E3" s="12">
         <f>DEGREES(ATAN2(B3,C3))</f>
-        <v>77.377398644331976</v>
+        <v>77.377558015175524</v>
       </c>
       <c r="G3" t="s">
         <v>58</v>
@@ -1450,72 +1456,72 @@
         <f>Sder/SQRT(3)/VTf</f>
         <v>231.49569734948909</v>
       </c>
-      <c r="M3">
-        <v>3.08342545</v>
+      <c r="K3">
+        <v>3.0834000000000001</v>
+      </c>
+      <c r="L3">
+        <v>2.2572999999999999</v>
       </c>
       <c r="N3">
-        <v>2.2573286000000001</v>
-      </c>
-      <c r="Q3">
-        <v>0.19290196515151514</v>
-      </c>
-      <c r="R3">
-        <v>0.86139753939393937</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+        <v>0.19289999999999999</v>
+      </c>
+      <c r="O3">
+        <v>0.86140000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="15">
-        <v>0.31714438939393941</v>
+        <v>0.31709999999999999</v>
       </c>
       <c r="C4" s="15">
-        <v>1.2826096606060606</v>
+        <v>1.2826</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ref="D4:D5" si="0">SQRT(B4*B4+C4*C4)</f>
-        <v>1.3212373387109708</v>
+        <v>1.3212173061234098</v>
       </c>
       <c r="E4" s="12">
         <f t="shared" ref="E4:E5" si="1">DEGREES(ATAN2(B4,C4))</f>
-        <v>76.111340974296184</v>
-      </c>
-      <c r="M4">
-        <v>4.16042545</v>
+        <v>76.11310912065909</v>
+      </c>
+      <c r="K4">
+        <v>4.1604000000000001</v>
+      </c>
+      <c r="L4">
+        <v>5.4843000000000002</v>
       </c>
       <c r="N4">
-        <v>5.4843286000000004</v>
-      </c>
-      <c r="Q4">
-        <v>0.31714438939393941</v>
-      </c>
-      <c r="R4">
-        <v>1.2826096606060606</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+        <v>0.31709999999999999</v>
+      </c>
+      <c r="O4">
+        <v>1.2826</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5" s="3">
         <f>(2*B3+B4)/3</f>
-        <v>0.23431610656565657</v>
+        <v>0.23429999999999998</v>
       </c>
       <c r="C5" s="3">
         <f>(2*C3+C4)/3</f>
-        <v>1.0018015797979798</v>
+        <v>1.0018</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="0"/>
-        <v>1.0288393669965279</v>
+        <v>1.0288341605914921</v>
       </c>
       <c r="E5" s="12">
         <f t="shared" si="1"/>
-        <v>76.835476832401341</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
+        <v>76.83633019769276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="B6" s="14" t="s">
         <v>51</v>
       </c>
@@ -1529,28 +1535,28 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>66</v>
       </c>
       <c r="B7" s="12">
         <f>VTf/SQRT(3)/D5</f>
-        <v>6997.7472555430813</v>
+        <v>6997.7826675734605</v>
       </c>
       <c r="C7" s="12">
         <f>-E5</f>
-        <v>-76.835476832401341</v>
+        <v>-76.83633019769276</v>
       </c>
       <c r="D7" s="12">
         <f>$B7*COS(RADIANS($C7))</f>
-        <v>1593.7229311472265</v>
+        <v>1593.629509803447</v>
       </c>
       <c r="E7" s="12">
         <f>$B7*SIN(RADIANS($C7))</f>
-        <v>-6813.8472151345031</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+        <v>-6813.9054328685224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1571,7 +1577,7 @@
         <v>-1153.0739316530619</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -1592,35 +1598,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>70</v>
       </c>
       <c r="B12" s="12">
         <f>B7+B8</f>
-        <v>8155.2257422905268</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+        <v>8155.2611543209059</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>69</v>
       </c>
       <c r="B13" s="12">
         <f>B7+B9</f>
-        <v>7275.5420923624679</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
+        <v>7275.577504392847</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:15">
       <c r="B16" s="14" t="s">
         <v>53</v>
       </c>
@@ -1640,19 +1646,19 @@
       </c>
       <c r="B17" s="12">
         <f>D7+D8</f>
-        <v>1694.6038283741354</v>
+        <v>1694.510407030356</v>
       </c>
       <c r="C17" s="12">
         <f>E7+E8</f>
-        <v>-7966.9211467875648</v>
+        <v>-7966.9793645215841</v>
       </c>
       <c r="D17" s="12">
         <f>SQRT(B17*B17+C17*C17)</f>
-        <v>8145.15283431018</v>
+        <v>8145.1903424196862</v>
       </c>
       <c r="E17" s="12">
         <f>DEGREES(ATAN2(B17,C17))</f>
-        <v>-77.991863922075368</v>
+        <v>-77.992591897977675</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1661,19 +1667,19 @@
       </c>
       <c r="B18" s="12">
         <f>D7+D9</f>
-        <v>1871.5177679666135</v>
+        <v>1871.424346622834</v>
       </c>
       <c r="C18" s="12">
         <f>E7+E9</f>
-        <v>-6813.8472151345031</v>
+        <v>-6813.9054328685224</v>
       </c>
       <c r="D18" s="12">
         <f>SQRT(B18*B18+C18*C18)</f>
-        <v>7066.1936448848437</v>
+        <v>7066.2250412230624</v>
       </c>
       <c r="E18" s="12">
         <f>DEGREES(ATAN2(B18,C18))</f>
-        <v>-74.641654114679824</v>
+        <v>-74.642509586294082</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1695,11 +1701,11 @@
       </c>
       <c r="B22" s="16">
         <f>B12/D17-1</f>
-        <v>1.2366751349239813E-3</v>
+        <v>1.2364121006198658E-3</v>
       </c>
       <c r="C22" s="16">
         <f>(B12-B7)/(D17-B7)-1</f>
-        <v>8.778855678190256E-3</v>
+        <v>8.7770128455602059E-3</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1708,11 +1714,11 @@
       </c>
       <c r="B23" s="16">
         <f>B13/D18-1</f>
-        <v>2.9626763431422454E-2</v>
+        <v>2.9627200088938599E-2</v>
       </c>
       <c r="C23" s="16">
         <f>(B13-B7)/(D18-B7)-1</f>
-        <v>3.0585754703921371</v>
+        <v>3.0588135975760729</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
include Z0 in the Figure B.4 screen shot
</commit_message>
<xml_diff>
--- a/HCA/SimpleRVC.xlsx
+++ b/HCA/SimpleRVC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\IEEE1729DynamicsTF\HCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BCFCB9-6F53-4E83-A4C8-61FDD46F6C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C92563A-CBF3-4AC7-B5E0-D0AE2BEAC0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="4290" windowWidth="14660" windowHeight="11160" xr2:uid="{7D6E8C32-CACD-498D-B92F-BBC7DE0016F8}"/>
+    <workbookView xWindow="4410" yWindow="3450" windowWidth="34060" windowHeight="16920" xr2:uid="{7D6E8C32-CACD-498D-B92F-BBC7DE0016F8}"/>
   </bookViews>
   <sheets>
     <sheet name="RVC" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="75">
   <si>
     <t>Linecode</t>
   </si>
@@ -573,6 +573,9 @@
       </rPr>
       <t>slgf</t>
     </r>
+  </si>
+  <si>
+    <t>Grounding Calculations</t>
   </si>
 </sst>
 </file>
@@ -583,7 +586,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,6 +648,15 @@
       <family val="1"/>
       <charset val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -679,7 +691,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -705,6 +717,7 @@
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,7 +1036,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1031,6 +1044,10 @@
     <col min="1" max="1" width="9.26953125" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.453125" customWidth="1"/>
+    <col min="7" max="7" width="2.54296875" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" customWidth="1"/>
+    <col min="10" max="10" width="7" customWidth="1"/>
+    <col min="11" max="11" width="7.08984375" customWidth="1"/>
     <col min="12" max="12" width="2.54296875" customWidth="1"/>
     <col min="13" max="13" width="2.36328125" customWidth="1"/>
   </cols>
@@ -1054,12 +1071,6 @@
       <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="5">
@@ -1082,16 +1093,8 @@
         <f>D2*$B2*$B2/$A2</f>
         <v>0.62200359999999999</v>
       </c>
-      <c r="I2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="3">
-        <f>E2</f>
-        <v>7.7750449999999999E-2</v>
-      </c>
-      <c r="K2" s="3">
-        <f>F2</f>
-        <v>0.62200359999999999</v>
+      <c r="H2" s="19" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -1107,11 +1110,11 @@
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>18</v>
+      <c r="J3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>62</v>
@@ -1141,19 +1144,16 @@
         <f t="shared" ref="F4:F5" si="1">$D4/5280*C4</f>
         <v>0.79</v>
       </c>
-      <c r="H4" s="3">
-        <v>0.63200000000000001</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1.744</v>
+      <c r="I4" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:K6" si="2">H4*$D4/5280</f>
-        <v>0.78999999999999992</v>
+        <f>E2</f>
+        <v>7.7750449999999999E-2</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" si="2"/>
-        <v>2.1799999999999997</v>
+        <f>F2</f>
+        <v>0.62200359999999999</v>
       </c>
       <c r="N4">
         <v>6600</v>
@@ -1183,19 +1183,11 @@
         <f t="shared" si="1"/>
         <v>0.63600000000000001</v>
       </c>
-      <c r="H5" s="3">
-        <v>2.3919999999999999</v>
-      </c>
-      <c r="I5" s="3">
-        <v>2.5680000000000001</v>
-      </c>
-      <c r="J5" s="3">
-        <f t="shared" si="2"/>
-        <v>1.794</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" si="2"/>
-        <v>1.9260000000000002</v>
+      <c r="H5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="N5">
         <v>3960</v>
@@ -1226,18 +1218,18 @@
         <v>0.20932500000000001</v>
       </c>
       <c r="H6" s="3">
-        <v>5.9946999999999999</v>
+        <v>0.63200000000000001</v>
       </c>
       <c r="I6" s="3">
-        <v>3.0253000000000001</v>
+        <v>1.744</v>
       </c>
       <c r="J6" s="3">
-        <f t="shared" si="2"/>
-        <v>1.498675</v>
+        <f>H6*$D4/5280</f>
+        <v>0.78999999999999992</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="2"/>
-        <v>0.75632500000000003</v>
+        <f>I6*$D4/5280</f>
+        <v>2.1799999999999997</v>
       </c>
       <c r="N6">
         <v>1320</v>
@@ -1258,16 +1250,19 @@
         <f>SUM(F2:F6)</f>
         <v>2.2573286000000001</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>22</v>
+      <c r="H7" s="3">
+        <v>2.3919999999999999</v>
+      </c>
+      <c r="I7" s="3">
+        <v>2.5680000000000001</v>
       </c>
       <c r="J7" s="3">
-        <f>SUM(J2:J6)</f>
-        <v>4.16042545</v>
+        <f>H7*$D5/5280</f>
+        <v>1.794</v>
       </c>
       <c r="K7" s="3">
-        <f>SUM(K2:K6)</f>
-        <v>5.4843286000000004</v>
+        <f>I7*$D5/5280</f>
+        <v>1.9260000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1277,15 +1272,19 @@
       <c r="B8" s="5">
         <v>12470</v>
       </c>
-      <c r="H8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" s="12">
-        <f>K7/F7</f>
-        <v>2.4295659036969628</v>
-      </c>
-      <c r="K8" t="s">
-        <v>46</v>
+      <c r="H8" s="3">
+        <v>5.9946999999999999</v>
+      </c>
+      <c r="I8" s="3">
+        <v>3.0253000000000001</v>
+      </c>
+      <c r="J8" s="3">
+        <f>H8*$D6/5280</f>
+        <v>1.498675</v>
+      </c>
+      <c r="K8" s="3">
+        <f>I8*$D6/5280</f>
+        <v>0.75632500000000003</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1302,15 +1301,16 @@
         <f>VT*VT+RG*DP+XG*DQ</f>
         <v>158343818.2649</v>
       </c>
-      <c r="H9" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" s="12">
-        <f>J7/F7</f>
-        <v>1.8430747964651668</v>
-      </c>
-      <c r="K9" t="s">
-        <v>47</v>
+      <c r="I9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="3">
+        <f>SUM(J4:J8)</f>
+        <v>4.16042545</v>
+      </c>
+      <c r="K9" s="3">
+        <f>SUM(K4:K8)</f>
+        <v>5.4843286000000004</v>
       </c>
       <c r="N9" s="17">
         <v>922000</v>
@@ -1332,6 +1332,28 @@
       <c r="E10" s="10">
         <f>XG*DP-RG*DQ</f>
         <v>2081256.9692000002</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="12">
+        <f>K9/F7</f>
+        <v>2.4295659036969628</v>
+      </c>
+      <c r="K10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="12">
+        <f>J9/F7</f>
+        <v>1.8430747964651668</v>
+      </c>
+      <c r="K11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:15">

</xml_diff>